<commit_message>
Added New Steps for Creating Journey Table
</commit_message>
<xml_diff>
--- a/Quroum_Round_USA/Stage1/StateToState.xlsx
+++ b/Quroum_Round_USA/Stage1/StateToState.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\A_Quorum_Journey\Quroum_Round_USA\Stage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\A_Quorum_Journey\Quroum_Round_USA\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9443F820-7236-4ED7-9542-678EB2ACD220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C7A76-83A1-4A30-A05D-9F853E91BD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3465" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="StatesCrossed" sheetId="2" r:id="rId2"/>
+    <sheet name="Stage2StatesCrossed" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$63</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="71">
   <si>
     <t>Order</t>
   </si>
@@ -245,12 +246,21 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000000000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -294,27 +304,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -322,7 +317,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -605,16 +601,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -996,7 +991,7 @@
         <v>-83.488986612365693</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1018,8 +1013,13 @@
       <c r="G17">
         <v>-84.522588056208903</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>2881</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1041,8 +1041,13 @@
       <c r="G18">
         <v>-86.742701181258795</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>7964</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1064,8 +1069,13 @@
       <c r="G19">
         <v>-87.519192946420205</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>9551</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1087,8 +1097,13 @@
       <c r="G20">
         <v>-90.182592462229394</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>11171</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1110,8 +1125,13 @@
       <c r="G21">
         <v>-94.607139544148794</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>13056</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1131,7 +1151,7 @@
         <v>-94.908508856479003</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1153,8 +1173,13 @@
       <c r="G23">
         <v>-93.937174543461893</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>14256</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1177,7 +1202,7 @@
         <v>-90.636798025705204</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1200,7 +1225,7 @@
         <v>-92.759555089986705</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1220,7 +1245,7 @@
         <v>-95.683511273435201</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1243,7 +1268,7 @@
         <v>-96.413737403750901</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1266,7 +1291,7 @@
         <v>-98.885590099601202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1289,7 +1314,7 @@
         <v>-104.05617915281999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1312,7 +1337,7 @@
         <v>-104.365954969264</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1335,7 +1360,7 @@
         <v>-115.695198922518</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1928,10 +1953,10 @@
       <c r="C58" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="6" t="s">
         <v>64</v>
       </c>
       <c r="F58">
@@ -2068,7 +2093,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,4 +2430,188 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F28B7B-C043-471C-A8B9-94B5D0E32AE0}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5">
+        <v>39.0922100114255</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-84.522588056208903</v>
+      </c>
+      <c r="F2">
+        <v>2881</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES ("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;")"</f>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (16,'Ohio ','Kentucky',39.0922100114255,-84.5225880562089,2881)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5">
+        <v>37.904329138035799</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-86.742701181258795</v>
+      </c>
+      <c r="F3">
+        <v>7964</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" si="0">"INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES ("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;")"</f>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (17,'Kentucky','Indiana',37.9043291380358,-86.7427011812588,7964)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5">
+        <v>38.7074572585826</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-87.519192946420205</v>
+      </c>
+      <c r="F4">
+        <v>9551</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (18,'Indiana','Illinois',38.7074572585826,-87.5191929464202,9551)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5">
+        <v>38.618003212465702</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-90.182592462229394</v>
+      </c>
+      <c r="F5">
+        <v>11171</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (19,'Illinois','Missouri',38.6180032124657,-90.1825924622294,11171)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="5">
+        <v>39.099016497713002</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-94.607139544148794</v>
+      </c>
+      <c r="F6">
+        <v>13056</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (20,'Missouri','Kansas',39.099016497713,-94.6071395441488,13056)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5">
+        <v>40.575218586784899</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-93.937174543461893</v>
+      </c>
+      <c r="F7">
+        <v>14256</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [dbo].[Journey_USA_States] ([Order],[ExitingState],[EnteringState],[Lat],[Lon] ,[Idx]) VALUES (22,'Missouri','Iowa',40.5752185867849,-93.9371745434619,14256)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>